<commit_message>
method shearch string ReadFile Ok
</commit_message>
<xml_diff>
--- a/planning/Calendar.xlsx
+++ b/planning/Calendar.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="440" windowWidth="33600" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="-33600" yWindow="-620" windowWidth="33600" windowHeight="20480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Semestres" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Nom</t>
   </si>
@@ -101,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -119,6 +119,20 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -234,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -244,34 +258,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -281,27 +280,37 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,100 +592,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="3" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
     <col min="4" max="5" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D2" s="5" t="s">
+    <row r="2" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="17"/>
+      <c r="C2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="25" t="s">
+    <row r="3" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="20">
         <v>42989</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="20">
         <v>43122</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="26"/>
-      <c r="C4" s="9" t="s">
+    <row r="4" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="25"/>
+      <c r="C4" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="21">
         <v>43122</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="20">
         <v>43255</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="27" t="s">
+    <row r="5" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="20">
         <v>42989</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>43122</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="26"/>
-      <c r="C6" s="20" t="s">
+    <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="25"/>
+      <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="16">
+      <c r="D6" s="21">
         <v>43122</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="20">
         <v>43255</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="28" t="s">
+    <row r="7" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="20">
         <v>42989</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <v>43122</v>
       </c>
     </row>
-    <row r="8" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="26"/>
-      <c r="C8" s="24" t="s">
+    <row r="8" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="25"/>
+      <c r="C8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="20">
         <v>43122</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="20">
         <v>43198</v>
       </c>
     </row>
@@ -694,7 +708,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -718,10 +734,10 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>43038</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>43045</v>
       </c>
     </row>
@@ -729,10 +745,10 @@
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>43094</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>43108</v>
       </c>
     </row>
@@ -740,21 +756,21 @@
       <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>43157</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>43164</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>43213</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>43227</v>
       </c>
     </row>
@@ -767,7 +783,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -791,10 +809,10 @@
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>42998</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="11">
         <v>2</v>
       </c>
     </row>
@@ -802,10 +820,10 @@
       <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>43055</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="11">
         <v>4</v>
       </c>
     </row>
@@ -813,206 +831,206 @@
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>43077</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="11">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="1"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C7" s="19"/>
-      <c r="D7" s="21"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
     </row>
     <row r="8" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C8" s="19"/>
-      <c r="D8" s="21"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
     </row>
     <row r="9" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C9" s="19"/>
-      <c r="D9" s="21"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
     </row>
     <row r="10" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C10" s="19"/>
-      <c r="D10" s="21"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
     </row>
     <row r="11" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C11" s="19"/>
-      <c r="D11" s="21"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C12" s="19"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C13" s="19"/>
-      <c r="D13" s="21"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C14" s="19"/>
-      <c r="D14" s="21"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C15" s="19"/>
-      <c r="D15" s="21"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C16" s="19"/>
-      <c r="D16" s="21"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C17" s="19"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C18" s="19"/>
-      <c r="D18" s="21"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C19" s="19"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C20" s="19"/>
-      <c r="D20" s="21"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C21" s="19"/>
-      <c r="D21" s="21"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
     </row>
     <row r="22" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C22" s="19"/>
-      <c r="D22" s="21"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C23" s="19"/>
-      <c r="D23" s="21"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="15"/>
     </row>
     <row r="24" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C24" s="19"/>
-      <c r="D24" s="21"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C25" s="23"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C26" s="23"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C27" s="23"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C28" s="23"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C29" s="23"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C30" s="23"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C31" s="23"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C32" s="23"/>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C33" s="23"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C34" s="23"/>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C35" s="23"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C36" s="23"/>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C37" s="23"/>
+      <c r="C37" s="16"/>
     </row>
     <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C38" s="23"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C39" s="23"/>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C40" s="23"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C41" s="23"/>
+      <c r="C41" s="16"/>
     </row>
     <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C42" s="23"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C43" s="23"/>
+      <c r="C43" s="16"/>
     </row>
     <row r="44" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C44" s="23"/>
+      <c r="C44" s="16"/>
     </row>
     <row r="45" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C45" s="23"/>
+      <c r="C45" s="16"/>
     </row>
     <row r="46" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C46" s="23"/>
+      <c r="C46" s="16"/>
     </row>
     <row r="47" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C47" s="23"/>
+      <c r="C47" s="16"/>
     </row>
     <row r="48" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C48" s="23"/>
+      <c r="C48" s="16"/>
     </row>
     <row r="49" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C49" s="23"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C50" s="23"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C51" s="23"/>
+      <c r="C51" s="16"/>
     </row>
     <row r="52" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C52" s="23"/>
+      <c r="C52" s="16"/>
     </row>
     <row r="53" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C53" s="23"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C54" s="23"/>
+      <c r="C54" s="16"/>
     </row>
     <row r="55" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C55" s="23"/>
+      <c r="C55" s="16"/>
     </row>
     <row r="56" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C56" s="23"/>
+      <c r="C56" s="16"/>
     </row>
     <row r="57" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C57" s="23"/>
+      <c r="C57" s="16"/>
     </row>
     <row r="58" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C58" s="23"/>
+      <c r="C58" s="16"/>
     </row>
     <row r="59" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C59" s="23"/>
+      <c r="C59" s="16"/>
     </row>
     <row r="60" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C60" s="23"/>
+      <c r="C60" s="16"/>
     </row>
     <row r="61" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C61" s="23"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C62" s="23"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" spans="3:3" ht="13" x14ac:dyDescent="0.15">
-      <c r="C63" s="23"/>
+      <c r="C63" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>